<commit_message>
Added tests for loading Excel file.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36A4332-ACDF-DE48-849B-9F71CBB2F53B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD9C84E-9527-D44A-AA96-D95704816B47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Case</t>
   </si>
@@ -94,12 +94,6 @@
   </si>
   <si>
     <t>t_star</t>
-  </si>
-  <si>
-    <t>R_orig</t>
-  </si>
-  <si>
-    <t>R_star</t>
   </si>
   <si>
     <t>eps_qo_M</t>
@@ -467,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -479,10 +473,10 @@
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,10 +505,10 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
@@ -526,28 +520,22 @@
         <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -591,29 +579,23 @@
         <v>31381</v>
       </c>
       <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
         <v>7</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="P2" s="1">
         <f>34444</f>
         <v>34444</v>
       </c>
-      <c r="R2" s="1">
-        <v>4007</v>
+      <c r="Q2" s="2">
+        <v>7</v>
+      </c>
+      <c r="R2" s="2">
+        <v>2861.13425677328</v>
       </c>
       <c r="S2" s="2">
-        <v>7</v>
-      </c>
-      <c r="T2" s="2">
-        <v>2861.13425677328</v>
-      </c>
-      <c r="U2" s="2">
         <v>2774.6681207909455</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -657,24 +639,18 @@
         <v>1.88</v>
       </c>
       <c r="O3" s="2">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="P3" s="2">
-        <v>1.8</v>
+        <v>1.21</v>
       </c>
       <c r="Q3" s="2">
-        <v>1.21</v>
+        <v>10</v>
       </c>
       <c r="R3" s="2">
         <v>0</v>
       </c>
       <c r="S3" s="2">
-        <v>10</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Splitting to orig, star, hat, bar, tilde functions.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D6913-2FE6-FB4B-834E-8D36C25ECADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB637A4F-A1CB-CC4F-BA0A-5C5680FA182C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1103,13 +1103,13 @@
     <t>MJ/engr_unit</t>
   </si>
   <si>
-    <t>e_ps_qs_UC</t>
-  </si>
-  <si>
     <t>e_qs_M</t>
   </si>
   <si>
     <t>e_qo_M</t>
+  </si>
+  <si>
+    <t>e_qs_ps_UC</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1539,13 +1539,13 @@
         <v>21</v>
       </c>
       <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>27</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Now calculating star variables.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB637A4F-A1CB-CC4F-BA0A-5C5680FA182C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190052F8-0805-CE4B-AF40-8A7F17057D26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1091,9 +1091,6 @@
     <t>eta_orig_engr_units</t>
   </si>
   <si>
-    <t>eta_tilde_engr_units</t>
-  </si>
-  <si>
     <t>E_emb_orig</t>
   </si>
   <si>
@@ -1110,6 +1107,9 @@
   </si>
   <si>
     <t>e_qs_ps_UC</t>
+  </si>
+  <si>
+    <t>eta_star_engr_units</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1495,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1521,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>14</v>
@@ -1536,16 +1536,16 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1572,10 +1572,10 @@
         <v>15</v>
       </c>
       <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
         <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:22">

</xml_diff>

<commit_message>
Adjusted for 2 times, ownership and lifetime.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190052F8-0805-CE4B-AF40-8A7F17057D26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9530B2-68F5-6E42-A01B-F65D7FB7EBB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>Matthew Heun</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
       <text>
         <r>
           <rPr>
@@ -195,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
       <text>
         <r>
           <rPr>
@@ -228,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
       <text>
         <r>
           <rPr>
@@ -261,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
       <text>
         <r>
           <rPr>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
       <text>
         <r>
           <rPr>
@@ -327,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
       <text>
         <r>
           <rPr>
@@ -360,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
       <text>
         <r>
           <rPr>
@@ -393,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
       <text>
         <r>
           <rPr>
@@ -426,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
       <text>
         <r>
           <rPr>
@@ -459,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
       <text>
         <r>
           <rPr>
@@ -492,7 +492,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
       <text>
         <r>
           <rPr>
@@ -525,7 +558,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
       <text>
         <r>
           <rPr>
@@ -558,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
       <text>
         <r>
           <rPr>
@@ -591,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
       <text>
         <r>
           <rPr>
@@ -624,7 +690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{E1AF7B22-FBF5-8F4E-B100-E76FDA62CB3C}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{E1AF7B22-FBF5-8F4E-B100-E76FDA62CB3C}">
       <text>
         <r>
           <rPr>
@@ -657,7 +723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
       <text>
         <r>
           <rPr>
@@ -690,7 +756,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
       <text>
         <r>
           <rPr>
@@ -723,7 +789,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
       <text>
         <r>
           <rPr>
@@ -756,7 +822,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
       <text>
         <r>
           <rPr>
@@ -790,7 +856,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
       <text>
         <r>
           <rPr>
@@ -823,7 +889,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
       <text>
         <r>
           <rPr>
@@ -856,7 +922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
       <text>
         <r>
           <rPr>
@@ -889,7 +955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
       <text>
         <r>
           <rPr>
@@ -922,7 +988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
       <text>
         <r>
           <rPr>
@@ -955,7 +1021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
       <text>
         <r>
           <rPr>
@@ -988,7 +1054,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
       <text>
         <r>
           <rPr>
@@ -1018,6 +1117,39 @@
             <family val="2"/>
           </rPr>
           <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
         </r>
       </text>
     </comment>
@@ -1026,7 +1158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Case</t>
   </si>
@@ -1079,15 +1211,9 @@
     <t>C_cap_orig</t>
   </si>
   <si>
-    <t>t_orig</t>
-  </si>
-  <si>
     <t>C_cap_star</t>
   </si>
   <si>
-    <t>t_star</t>
-  </si>
-  <si>
     <t>eta_orig_engr_units</t>
   </si>
   <si>
@@ -1110,13 +1236,31 @@
   </si>
   <si>
     <t>eta_star_engr_units</t>
+  </si>
+  <si>
+    <t>t_own_orig</t>
+  </si>
+  <si>
+    <t>t_own_star</t>
+  </si>
+  <si>
+    <t>t_life_orig</t>
+  </si>
+  <si>
+    <t>t_life_star</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>None yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1492,226 +1636,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
       </c>
       <c r="L1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.7453574085249099E-2</v>
+      </c>
+      <c r="I2" s="2">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>126.62163000000001</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3.3893390630606466</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1.7453574085249099E-2</v>
-      </c>
-      <c r="H2" s="2">
-        <v>25</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>42</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>-0.1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
         <v>14425</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>27401.277693029457</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>28216.1</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>7</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>27523.4</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>7</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>2861.13425677328</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>2774.6681207909455</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>34000</v>
       </c>
-      <c r="V2">
+      <c r="W2">
+        <v>14</v>
+      </c>
+      <c r="X2">
         <v>40000</v>
       </c>
+      <c r="Y2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>3.6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>3.3893390630606466</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>3.7638919000000007E-2</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>8833.3333333333303</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>81800</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>-0.4</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
       </c>
       <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
         <v>580350</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>27401.277693029457</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>1.88</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>1.8</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>1.21</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>10</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
       </c>
       <c r="T3" s="2">
         <v>0</v>
       </c>
       <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="X3" s="2">
         <v>6.5</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first indifference curve.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7158E0-2F36-D94D-96B0-490A51841737}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27230B-FEF8-BF4E-8D9A-B5212EDE3ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1638,8 +1638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Adding engr units to input table.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF27230B-FEF8-BF4E-8D9A-B5212EDE3ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56CE73F-FB32-5648-B22E-E1AD15905E83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -30,7 +30,106 @@
     <author>Matthew Heun</author>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{177A5939-9C5C-134F-8638-CA4D7AC90D6E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the unit of the numerator of the efficiency terms.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E7917100-B885-C647-B060-CE8FA6C0FA9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This is the unit of denominator of the efficiency terms.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2E9F2B67-4158-6D4C-9AF8-868A6C525FDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This unit conversion factor translates from energy engineering units to MJ.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
       <text>
         <r>
           <rPr>
@@ -63,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{142CF5A0-F2F7-6049-8D23-3DC70BA56F2B}">
       <text>
         <r>
           <rPr>
@@ -96,40 +195,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/MJ</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{212DB243-4B09-8641-8DD9-2C5771F409BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/gal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{BD5F855E-F716-1C40-9BD9-51470AF65E6E}">
       <text>
         <r>
           <rPr>
@@ -162,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{724ED12C-E3B7-174A-AED0-FF81928555B3}">
       <text>
         <r>
           <rPr>
@@ -195,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{2E11DCDD-2255-D142-98F1-B4F74C45A04F}">
       <text>
         <r>
           <rPr>
@@ -228,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{30C499C2-FCE1-5541-A599-047491F4BB43}">
       <text>
         <r>
           <rPr>
@@ -261,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{15643D2B-90F6-2E4E-923B-C7BAE01F5865}">
       <text>
         <r>
           <rPr>
@@ -294,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
       <text>
         <r>
           <rPr>
@@ -327,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
       <text>
         <r>
           <rPr>
@@ -360,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
       <text>
         <r>
           <rPr>
@@ -393,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
       <text>
         <r>
           <rPr>
@@ -426,7 +525,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
       <text>
         <r>
           <rPr>
@@ -459,7 +558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
       <text>
         <r>
           <rPr>
@@ -492,7 +591,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
       <text>
         <r>
           <rPr>
@@ -525,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
       <text>
         <r>
           <rPr>
@@ -558,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
       <text>
         <r>
           <rPr>
@@ -591,7 +690,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
       <text>
         <r>
           <rPr>
@@ -624,7 +723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{71304EAD-8694-A043-956C-0A2C3D40E024}">
       <text>
         <r>
           <rPr>
@@ -657,106 +756,107 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/MJ</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{E1AF7B22-FBF5-8F4E-B100-E76FDA62CB3C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lumens/kW</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lumens/kW</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{49C83D03-F8EC-0A4D-B9F1-028C82EC8FB7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{3A848E02-53A6-E54E-8E01-9938DB10D028}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{A7BA69FC-7890-0148-8572-5FF6A4FC8660}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{2DC2CF3D-CB10-0447-A6BB-E13E504BFF4F}">
       <text>
         <r>
           <rPr>
@@ -789,7 +889,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{B210CA66-900D-DB4B-B4C2-AD78BD37EB4D}">
       <text>
         <r>
           <rPr>
@@ -822,7 +922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{ABF2326C-BA2D-BE47-8827-CD63D8839125}">
       <text>
         <r>
           <rPr>
@@ -856,7 +956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
       <text>
         <r>
           <rPr>
@@ -889,7 +989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
       <text>
         <r>
           <rPr>
@@ -922,7 +1022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
       <text>
         <r>
           <rPr>
@@ -955,7 +1055,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
       <text>
         <r>
           <rPr>
@@ -988,7 +1088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
       <text>
         <r>
           <rPr>
@@ -1021,7 +1121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{45DDB177-C1A1-5149-92E1-8111CF45C971}">
       <text>
         <r>
           <rPr>
@@ -1054,7 +1154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{29C5D0E3-585B-BC4A-B190-9798E0FAB668}">
       <text>
         <r>
           <rPr>
@@ -1087,7 +1187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{17F72B11-97B9-7B48-A64B-18186A392A64}">
       <text>
         <r>
           <rPr>
@@ -1120,7 +1220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{5CC62B9E-5447-4747-A121-4B743BE1C195}">
       <text>
         <r>
           <rPr>
@@ -1158,7 +1258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Case</t>
   </si>
@@ -1172,9 +1272,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>p_E</t>
-  </si>
-  <si>
     <t>q_dot_s_orig</t>
   </si>
   <si>
@@ -1254,6 +1351,27 @@
   </si>
   <si>
     <t>Lamp</t>
+  </si>
+  <si>
+    <t>energy_engr_unit</t>
+  </si>
+  <si>
+    <t>gal</t>
+  </si>
+  <si>
+    <t>lm-hr</t>
+  </si>
+  <si>
+    <t>service_unit</t>
+  </si>
+  <si>
+    <t>miles</t>
+  </si>
+  <si>
+    <t>kW-hr</t>
+  </si>
+  <si>
+    <t>p_E_engr_units</t>
   </si>
 </sst>
 </file>
@@ -1636,27 +1754,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W30" sqref="W30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1668,220 +1788,238 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>21</v>
       </c>
       <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2.21</v>
+      </c>
+      <c r="K2" s="2">
         <v>25</v>
       </c>
-      <c r="T1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3">
-        <v>126.62163000000001</v>
-      </c>
-      <c r="F2" s="2">
-        <v>3.3893390630606466</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="L2" s="2">
+        <v>42</v>
+      </c>
+      <c r="M2" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="N2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="2">
-        <v>1.7453574085249099E-2</v>
-      </c>
-      <c r="I2" s="2">
-        <v>25</v>
-      </c>
-      <c r="J2" s="2">
-        <v>42</v>
-      </c>
-      <c r="K2" s="2">
-        <v>-0.1</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="P2" s="2">
         <v>14425</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>27401.277693029457</v>
       </c>
-      <c r="P2" s="2">
+      <c r="R2" s="2">
         <v>28216.1</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>7</v>
-      </c>
-      <c r="R2" s="1">
-        <v>27523.4</v>
       </c>
       <c r="S2" s="2">
         <v>7</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
+        <v>27523.4</v>
+      </c>
+      <c r="U2" s="2">
+        <v>7</v>
+      </c>
+      <c r="V2" s="2">
         <v>2861.13425677328</v>
       </c>
-      <c r="U2" s="2">
+      <c r="W2" s="2">
         <v>2774.6681207909455</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>34000</v>
-      </c>
-      <c r="W2">
-        <v>14</v>
-      </c>
-      <c r="X2">
-        <v>40000</v>
       </c>
       <c r="Y2">
         <v>14</v>
       </c>
+      <c r="Z2">
+        <v>40000</v>
+      </c>
+      <c r="AA2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3">
         <v>3.6</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <v>3.3893390630606466</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
-        <v>3.7638919000000007E-2</v>
-      </c>
-      <c r="I3" s="4">
+      <c r="J3" s="2">
+        <v>0.13550000000000001</v>
+      </c>
+      <c r="K3" s="4">
         <v>8833.3333333333303</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>81800</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>-0.4</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>580350</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>27401.277693029457</v>
       </c>
-      <c r="P3" s="2">
+      <c r="R3" s="2">
         <v>1.88</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="S3" s="2">
         <v>1.8</v>
       </c>
-      <c r="R3" s="2">
+      <c r="T3" s="2">
         <v>1.21</v>
       </c>
-      <c r="S3" s="2">
+      <c r="U3" s="2">
         <v>10</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <v>0</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <v>0</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <v>1.8</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Z3" s="2">
         <v>6.5</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="AA3" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding elasticity names to constants.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/ReboundTools/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4E3F61-8AEF-544B-8CAC-F8C5757350D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB1E59-626A-EE49-A68E-D2C9F3D0C623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23180" yWindow="460" windowWidth="26260" windowHeight="16940" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
@@ -1417,9 +1417,6 @@
     <t>e_qo_M</t>
   </si>
   <si>
-    <t>e_qs_ps_UC</t>
-  </si>
-  <si>
     <t>t_own_orig</t>
   </si>
   <si>
@@ -1472,6 +1469,9 @@
   </si>
   <si>
     <t>W-hr</t>
+  </si>
+  <si>
+    <t>e_qs_ps_UC_orig</t>
   </si>
 </sst>
 </file>
@@ -1534,11 +1534,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1558,7 +1555,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1846,7 +1843,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1856,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1876,7 +1873,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1888,13 +1885,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -1903,10 +1900,10 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="L1" t="s">
         <v>17</v>
@@ -1915,10 +1912,10 @@
         <v>18</v>
       </c>
       <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
         <v>33</v>
-      </c>
-      <c r="O1" t="s">
-        <v>34</v>
       </c>
       <c r="P1" t="s">
         <v>4</v>
@@ -1930,13 +1927,13 @@
         <v>13</v>
       </c>
       <c r="S1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T1" t="s">
         <v>14</v>
       </c>
       <c r="U1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
         <v>5</v>
@@ -1948,83 +1945,83 @@
         <v>15</v>
       </c>
       <c r="Y1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z1" t="s">
         <v>16</v>
       </c>
       <c r="AA1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
         <v>126.62163000000001</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>3.3893390630606466</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>2.21</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>-0.1</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2">
         <v>25</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>42</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>14425</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2">
         <v>27401.277693029457</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2">
         <v>28216.1</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2">
         <v>7</v>
       </c>
       <c r="T2" s="1">
         <v>27523.4</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2">
         <v>7</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2">
         <v>2861.13425677328</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2">
         <v>2774.6681207909455</v>
       </c>
       <c r="X2">
@@ -2042,91 +2039,89 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>3.3893390630606466</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>1.3549999999999999E-4</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>-0.4</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="1">
         <v>8.8333332999999996</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3">
         <v>81.8</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3">
         <v>580350</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3">
         <v>27401.277693029457</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3">
         <v>1.88</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3">
         <v>1.8</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3">
         <v>1.21</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3">
         <v>10</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3">
         <v>0</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3">
         <v>0</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3">
         <v>1.8</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3">
         <v>6.5</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="J4" s="2"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
+      <c r="N4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Now including the r column
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FB1E59-626A-EE49-A68E-D2C9F3D0C623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F47EBFD-5AA4-CA44-923B-51689101ACD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Matthew Heun</author>
+    <author>Matt</author>
   </authors>
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{177A5939-9C5C-134F-8638-CA4D7AC90D6E}">
@@ -129,6 +130,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="AB1" authorId="1" shapeId="0" xr:uid="{6A2BC25A-23CC-EA47-B649-1DF6A69EAC05}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Discount rate for R calculations.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G2" authorId="0" shapeId="0" xr:uid="{9482D8EB-43D3-CD42-B9A3-577AD33D043C}">
       <text>
         <r>
@@ -690,6 +724,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="AB2" authorId="1" shapeId="0" xr:uid="{D3207F3D-4460-E648-909E-B295908D812B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1/yr</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G3" authorId="0" shapeId="0" xr:uid="{887A79FC-140D-2443-8496-3599E39BA9B7}">
       <text>
         <r>
@@ -1250,6 +1317,39 @@
             <family val="2"/>
           </rPr>
           <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB3" authorId="1" shapeId="0" xr:uid="{45008C01-ABF6-7F4C-9EEB-2980C7E38C4E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1/yr</t>
         </r>
       </text>
     </comment>
@@ -1358,7 +1458,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Case</t>
   </si>
@@ -1472,6 +1572,9 @@
   </si>
   <si>
     <t>e_qs_ps_UC_orig</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -1555,9 +1658,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1595,7 +1698,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1701,7 +1804,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1843,7 +1946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1851,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1871,7 +1974,7 @@
     <col min="22" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1953,8 +2056,11 @@
       <c r="AA1" t="s">
         <v>22</v>
       </c>
+      <c r="AB1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2036,8 +2142,11 @@
       <c r="AA2">
         <v>14</v>
       </c>
+      <c r="AB2">
+        <v>0.03</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2119,8 +2228,11 @@
       <c r="AA3">
         <v>10</v>
       </c>
+      <c r="AB3">
+        <v>0.03</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="N4" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got original calculations working.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC04B4F-7F7E-9841-9D14-54368940805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56D9153-6A63-6D40-A758-0FBB6A5F2BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -460,40 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
+    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
       <text>
         <r>
           <rPr>
@@ -526,40 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
+    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
       <text>
         <r>
           <rPr>
@@ -592,7 +537,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="1" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
+    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{FE77101E-623C-924A-AC94-2312199C6D09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Disposal cost at end of life, $</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
       <text>
         <r>
           <rPr>
@@ -625,6 +603,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="X2" authorId="1" shapeId="0" xr:uid="{8A754275-DD66-B649-9461-3B777D2F2C2E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Disposal cost at end of life, $</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Y2" authorId="1" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
       <text>
         <r>
@@ -1056,40 +1068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="1" shapeId="0" xr:uid="{38DCB468-6D7F-484A-A8F8-EBEF999C7AED}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U3" authorId="1" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
+    <comment ref="T3" authorId="1" shapeId="0" xr:uid="{DF64169F-D5C4-EF48-A273-4073182699CB}">
       <text>
         <r>
           <rPr>
@@ -1122,40 +1101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="1" shapeId="0" xr:uid="{FE70D0C3-F2E6-E243-8896-EB0C92299AD5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W3" authorId="1" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
+    <comment ref="U3" authorId="1" shapeId="0" xr:uid="{FFC2A0D3-7A2D-CE4D-83FD-FDA9B4B45B38}">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1134,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="1" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
+    <comment ref="V3" authorId="1" shapeId="0" xr:uid="{B72D4129-305A-9048-BEE7-C71523D7FFA2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Disposal cost at end of life, $</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W3" authorId="1" shapeId="0" xr:uid="{28F2D47D-E587-9642-9506-677918A4E61E}">
       <text>
         <r>
           <rPr>
@@ -1218,6 +1197,40 @@
             <family val="2"/>
           </rPr>
           <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X3" authorId="1" shapeId="0" xr:uid="{7803960F-DCE2-AF4B-80E8-5E160CE73CA3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Disposal cost at end of life, $</t>
         </r>
       </text>
     </comment>
@@ -1475,9 +1488,6 @@
     <t>q_dot_s_orig</t>
   </si>
   <si>
-    <t>C_dot_md_orig</t>
-  </si>
-  <si>
     <t>M_dot_orig</t>
   </si>
   <si>
@@ -1496,9 +1506,6 @@
     <t>I_E</t>
   </si>
   <si>
-    <t>C_dot_md_star</t>
-  </si>
-  <si>
     <t>C_cap_orig</t>
   </si>
   <si>
@@ -1517,12 +1524,6 @@
     <t>e_qo_M</t>
   </si>
   <si>
-    <t>t_own_orig</t>
-  </si>
-  <si>
-    <t>t_own_star</t>
-  </si>
-  <si>
     <t>t_life_orig</t>
   </si>
   <si>
@@ -1575,6 +1576,18 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>C_dot_om_orig</t>
+  </si>
+  <si>
+    <t>C_d_orig</t>
+  </si>
+  <si>
+    <t>C_dot_om_star</t>
+  </si>
+  <si>
+    <t>C_d_star</t>
   </si>
 </sst>
 </file>
@@ -1956,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1971,12 +1984,15 @@
     <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1988,99 +2004,99 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Q1" t="s">
         <v>4</v>
       </c>
       <c r="R1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>16</v>
-      </c>
       <c r="AB1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2">
         <v>0.03</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H2">
         <v>126.62163000000001</v>
@@ -2118,20 +2134,20 @@
       <c r="S2">
         <v>28216.1</v>
       </c>
-      <c r="T2">
-        <v>7</v>
-      </c>
-      <c r="U2" s="1">
+      <c r="T2" s="1">
         <v>27523.4</v>
       </c>
+      <c r="U2">
+        <v>2861.13425677328</v>
+      </c>
       <c r="V2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>2861.13425677328</v>
+        <v>2774.6681207909455</v>
       </c>
       <c r="X2">
-        <v>2774.6681207909455</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <v>34000</v>
@@ -2148,25 +2164,25 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
       <c r="E3">
         <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H3">
         <v>3.5999999999999999E-3</v>
@@ -2205,13 +2221,13 @@
         <v>1.88</v>
       </c>
       <c r="T3">
-        <v>1.8</v>
+        <v>1.21</v>
       </c>
       <c r="U3">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <v>0</v>

</xml_diff>

<commit_message>
Fix tests when C_d is non-zero
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56D9153-6A63-6D40-A758-0FBB6A5F2BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D3ECB-35A1-F14D-BA1D-A8D244B1F11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -631,7 +631,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Disposal cost at end of life, $</t>
         </r>
@@ -1594,7 +1593,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1628,6 +1627,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1970,7 +1975,7 @@
   <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2141,13 +2146,13 @@
         <v>2861.13425677328</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W2">
         <v>2774.6681207909455</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="Y2">
         <v>34000</v>

</xml_diff>

<commit_message>
Getting r = 0 into tests.
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D3ECB-35A1-F14D-BA1D-A8D244B1F11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55044EC2-54FF-8A48-A793-B67512BB8A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -1365,73 +1365,436 @@
         </r>
       </text>
     </comment>
-    <comment ref="K4" authorId="1" shapeId="0" xr:uid="{85BAFE31-3780-1940-8E16-66F5E918C1C5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>$/kW-hr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="1" shapeId="0" xr:uid="{F8398967-746F-AB4D-B2CF-41C142C00435}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>lm-hr/kW-hr</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P4" authorId="1" shapeId="0" xr:uid="{1EBB8036-1BE2-CB40-90CF-91443588B8E4}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{FD980A4C-8F0D-284E-8254-F0D92A2F9FEE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="1" shapeId="0" xr:uid="{F6B65BEC-02A1-6640-9F3B-16993ACAF934}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="1" shapeId="0" xr:uid="{9F446724-6017-1241-A251-13CE14FD547F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="1" shapeId="0" xr:uid="{C766CBAE-7890-6248-AC01-E4CB8FDD3667}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/gal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="1" shapeId="0" xr:uid="{703C2B71-2DE0-FB41-8F58-F1817738D334}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P4" authorId="1" shapeId="0" xr:uid="{EBE5B3BC-FE25-3A43-8AA4-20AAA83216B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q4" authorId="1" shapeId="0" xr:uid="{D327AC31-8B3D-B344-AEAC-B28873FE8B3F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="1" shapeId="0" xr:uid="{65F05505-2BA9-B349-9B3E-D4F836CE3BE5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="1" shapeId="0" xr:uid="{EDF46648-4714-A244-92D2-B40B00A958BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="1" shapeId="0" xr:uid="{35D063AD-377F-784B-8D1C-8034339B3EB3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U4" authorId="1" shapeId="0" xr:uid="{458E7C53-73B4-A245-8125-F003D42FC026}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V4" authorId="1" shapeId="0" xr:uid="{665366B4-2AFD-0D4B-9840-543A71B584EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Disposal cost at end of life, $</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W4" authorId="1" shapeId="0" xr:uid="{91BA356B-BE9B-6E4D-B37C-25988B03C0D5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X4" authorId="1" shapeId="0" xr:uid="{5AE112F7-9DD4-F74E-A462-8A19A3B9DD98}">
       <text>
         <r>
           <rPr>
@@ -1459,9 +1822,140 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>lm-hr/kW-hr</t>
+          </rPr>
+          <t>Disposal cost at end of life, $</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="1" shapeId="0" xr:uid="{B8F934E5-12F0-D444-BB3D-9B2FCEFE2657}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z4" authorId="1" shapeId="0" xr:uid="{CD869F9D-832D-E949-841C-A73E44BED530}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA4" authorId="1" shapeId="0" xr:uid="{289AF292-1DE9-C544-A340-C51BBA0E7B39}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB4" authorId="1" shapeId="0" xr:uid="{FB2B46D7-4810-C949-A20A-208A74F29AB9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
         </r>
       </text>
     </comment>
@@ -1470,7 +1964,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Case</t>
   </si>
@@ -1587,6 +2081,9 @@
   </si>
   <si>
     <t>C_d_star</t>
+  </si>
+  <si>
+    <t>Car, r = 0</t>
   </si>
 </sst>
 </file>
@@ -1974,8 +2471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2254,7 +2751,90 @@
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="O4" s="1"/>
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="I4">
+        <v>3.3893390630606466</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>2.21</v>
+      </c>
+      <c r="L4">
+        <v>-0.1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>25</v>
+      </c>
+      <c r="P4">
+        <v>42</v>
+      </c>
+      <c r="Q4">
+        <v>14425</v>
+      </c>
+      <c r="R4">
+        <v>27401.277693029457</v>
+      </c>
+      <c r="S4">
+        <v>28216.1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>27523.4</v>
+      </c>
+      <c r="U4">
+        <v>2861.13425677328</v>
+      </c>
+      <c r="V4">
+        <v>100</v>
+      </c>
+      <c r="W4">
+        <v>2774.6681207909455</v>
+      </c>
+      <c r="X4">
+        <v>101</v>
+      </c>
+      <c r="Y4">
+        <v>34000</v>
+      </c>
+      <c r="Z4">
+        <v>14</v>
+      </c>
+      <c r="AA4">
+        <v>40000</v>
+      </c>
+      <c r="AB4">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More o --> g
</commit_message>
<xml_diff>
--- a/inst/extdata/example_eeu_data.xlsx
+++ b/inst/extdata/example_eeu_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundTools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55044EC2-54FF-8A48-A793-B67512BB8A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43A81AB-3B73-8B48-8F8D-404C6323D296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -2014,9 +2014,6 @@
     <t>e_qs_M</t>
   </si>
   <si>
-    <t>e_qo_M</t>
-  </si>
-  <si>
     <t>t_life_orig</t>
   </si>
   <si>
@@ -2084,6 +2081,9 @@
   </si>
   <si>
     <t>Car, r = 0</t>
+  </si>
+  <si>
+    <t>e_qg_M</t>
   </si>
 </sst>
 </file>
@@ -2471,8 +2471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2494,7 +2494,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2506,16 +2506,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
@@ -2524,22 +2524,22 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
         <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
       </c>
       <c r="Q1" t="s">
         <v>4</v>
@@ -2554,36 +2554,36 @@
         <v>12</v>
       </c>
       <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
-      </c>
-      <c r="X1" t="s">
-        <v>38</v>
       </c>
       <c r="Y1" t="s">
         <v>13</v>
       </c>
       <c r="Z1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA1" t="s">
         <v>14</v>
       </c>
       <c r="AB1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -2595,10 +2595,10 @@
         <v>0.03</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2">
         <v>126.62163000000001</v>
@@ -2666,10 +2666,10 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2681,10 +2681,10 @@
         <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>3.5999999999999999E-3</v>
@@ -2752,10 +2752,10 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -2767,10 +2767,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>126.62163000000001</v>

</xml_diff>